<commit_message>
feat: introduce Excel import functionality, add sales and supervisor dashboard charts, and update Vite configuration.
</commit_message>
<xml_diff>
--- a/public/file/template_input.xlsx
+++ b/public/file/template_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FAHD\Desktop\indonusa_project\public\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\F Project\Indonusa Project\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1829793-C97E-4BAB-BAD9-4F20FC63E9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544F7CFA-B29F-4CDC-B6E9-646C59B1275B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="10770" xr2:uid="{FF9404A3-B408-4DC3-B687-F8E2C50F4E09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FF9404A3-B408-4DC3-B687-F8E2C50F4E09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DESKRIPSI</t>
   </si>
@@ -34,21 +34,6 @@
   </si>
   <si>
     <t>HARGA</t>
-  </si>
-  <si>
-    <t>SPESIFIKASI</t>
-  </si>
-  <si>
-    <t>GAMBAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                     </t>
   </si>
   <si>
     <t>KATEGORI</t>
@@ -67,7 +52,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$Rp-3809]* #,##0.00_-;\-[$Rp-3809]* #,##0.00_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +66,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -124,13 +115,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent6" xfId="1" builtinId="49"/>
@@ -150,9 +142,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -190,7 +182,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -296,7 +288,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -438,7 +430,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,41 +438,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB230B3-8D72-4915-8BE9-78DBB97685C0}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
@@ -488,37 +479,18 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
       <c r="B2"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H20" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add client-side Excel upload functionality with header mapping, data validation, and unique product code generation, including a new template.
</commit_message>
<xml_diff>
--- a/public/file/template_input.xlsx
+++ b/public/file/template_input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\F Project\Indonusa Project\public\file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544F7CFA-B29F-4CDC-B6E9-646C59B1275B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C2AE99-70F8-44A1-A8DC-C10C6ED6B1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FF9404A3-B408-4DC3-B687-F8E2C50F4E09}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>DESKRIPSI</t>
   </si>
@@ -43,6 +43,96 @@
   </si>
   <si>
     <t>NAMA BARANG</t>
+  </si>
+  <si>
+    <t>MISCELLANEOUS</t>
+  </si>
+  <si>
+    <t>HANDTOOLS</t>
+  </si>
+  <si>
+    <t>LIST KATEGORI</t>
+  </si>
+  <si>
+    <t>ADHESIVE AND SEALANT</t>
+  </si>
+  <si>
+    <t>AUTOMOTIVE EQUIPMENT</t>
+  </si>
+  <si>
+    <t>CLEANING</t>
+  </si>
+  <si>
+    <t>COMPRESSOR</t>
+  </si>
+  <si>
+    <t>CONSTRUCTION</t>
+  </si>
+  <si>
+    <t>CUTTING TOOLS</t>
+  </si>
+  <si>
+    <t>LIGHTING</t>
+  </si>
+  <si>
+    <t>FASTENING</t>
+  </si>
+  <si>
+    <t>GENERATOR</t>
+  </si>
+  <si>
+    <t>HEALTH CARE EQUIPMENT</t>
+  </si>
+  <si>
+    <t>HOSPITALITY</t>
+  </si>
+  <si>
+    <t>HYDRAULIC TOOLS</t>
+  </si>
+  <si>
+    <t>MARKING MACHINE</t>
+  </si>
+  <si>
+    <t>MATERIAL HANDLING EQUIPMENT</t>
+  </si>
+  <si>
+    <t>MEASURING AND TESTING EQUIPMENT</t>
+  </si>
+  <si>
+    <t>METAL CUTTING MACHINERY</t>
+  </si>
+  <si>
+    <t>PACKAGING</t>
+  </si>
+  <si>
+    <t>PAINTING AND COATING</t>
+  </si>
+  <si>
+    <t>PNEUMATIC TOOLS</t>
+  </si>
+  <si>
+    <t>POWER TOOLS</t>
+  </si>
+  <si>
+    <t>SAFETY AND PROTECTION EQUIPMENT</t>
+  </si>
+  <si>
+    <t>SECURITY</t>
+  </si>
+  <si>
+    <t>SHEET METAL MACHINERY</t>
+  </si>
+  <si>
+    <t>STORAGE SYSTEM</t>
+  </si>
+  <si>
+    <t>WELDING EQUIPMENT</t>
+  </si>
+  <si>
+    <t>WOODWORKING EQUIPMENT</t>
+  </si>
+  <si>
+    <t>OTHER CATEGORIES</t>
   </si>
 </sst>
 </file>
@@ -52,7 +142,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$Rp-3809]* #,##0.00_-;\-[$Rp-3809]* #,##0.00_-;_-[$Rp-3809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,8 +163,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,8 +182,14 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -110,12 +212,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -123,6 +234,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent6" xfId="1" builtinId="49"/>
@@ -438,29 +553,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB230B3-8D72-4915-8BE9-78DBB97685C0}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="38.140625" customWidth="1"/>
     <col min="9" max="9" width="23.140625" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -479,17 +594,170 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2"/>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3"/>
       <c r="F3" s="3"/>
+      <c r="H3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4"/>
+      <c r="F4" s="3"/>
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{C302F719-4B6F-4D2C-A3F7-6CA449A06E60}">
+      <formula1>$H$2:$H$30</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>